<commit_message>
Revert "1.加入By Section Enable/Disable的功能"
This reverts commit 8283e1cef4018edb0d8155f390bce471dee242ed.
</commit_message>
<xml_diff>
--- a/BCWinForm/Config/SOUTH_INNOLUX/CSTTranSchedule.xlsx
+++ b/BCWinForm/Config/SOUTH_INNOLUX/CSTTranSchedule.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB7C1D32-0BED-F441-81F4-7D8D1E344251}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
     <sheet name="工作表1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2613" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="525">
   <si>
     <t>HOSTSOURCE</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1600,20 +1599,12 @@
   </si>
   <si>
     <t xml:space="preserve">AA1100                                  </t>
-  </si>
-  <si>
-    <t>STKT1300-B1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STKT1400-B2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
@@ -1952,82 +1943,478 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.19921875" style="2"/>
+    <col min="1" max="1" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:15">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>525</v>
+      <c r="B1" s="1">
+        <v>10001</v>
+      </c>
+      <c r="C1" s="1">
+        <v>10002</v>
+      </c>
+      <c r="D1" s="1">
+        <v>10003</v>
+      </c>
+      <c r="E1" s="1">
+        <v>10004</v>
+      </c>
+      <c r="F1" s="1">
+        <v>10005</v>
+      </c>
+      <c r="G1" s="1">
+        <v>10006</v>
+      </c>
+      <c r="H1" s="1">
+        <v>10007</v>
+      </c>
+      <c r="I1" s="1">
+        <v>10008</v>
+      </c>
+      <c r="J1" s="1">
+        <v>10009</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10010</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="1">
+        <v>10001</v>
       </c>
       <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>526</v>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="1">
+        <v>10002</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="1">
+        <v>10003</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1">
+        <v>10004</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1">
+        <v>10005</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1">
+        <v>10006</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1">
+        <v>10007</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1">
+        <v>10008</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1">
+        <v>10009</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1">
+        <v>10010</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2037,20 +2424,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E869"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="50.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>